<commit_message>
Change file structure and fix some bug
</commit_message>
<xml_diff>
--- a/conf/excel/C_BackPolygon.xlsx
+++ b/conf/excel/C_BackPolygon.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\配置文件相关\newCA-config-clear\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\配置文件相关\newCA-config-clear\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF2C504-B130-4400-984E-7682ADE5A81A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C_BackPolygon.conf" sheetId="1" r:id="rId1"/>
+    <sheet name="C_BackPolygon_Filter.conf" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'C_BackPolygon.conf'!$A$1:$C$77</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="227">
   <si>
     <r>
       <rPr>
@@ -807,11 +807,44 @@
     <t>catalog=090101057</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>&lt;Empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除机场相关的北京面防止背景面压盖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name != 北京首都国际机场 &amp;&amp; name != 上海浦东国际机场 &amp;&amp; name != 上海虹桥机场 &amp;&amp; name != 深圳宝安国际机场 &amp;&amp; name != 广州白云国际机场)$"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id != 40061876757 &amp;&amp; id != 40061876760 &amp;&amp; id != 40061876765 &amp;&amp; id != 40061876764 &amp;&amp; id != 40007284849 &amp;&amp; id != 40000293144 &amp;&amp; id != 40005694932 &amp;&amp; id != 40005694930</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t># C_BackPolygon</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（过滤使用）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,7 +934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -922,6 +955,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1203,11 +1245,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1218,18 +1260,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2079,7 +2121,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C77" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:C77">
     <filterColumn colId="0" showButton="0"/>
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
@@ -2091,4 +2133,82 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.875" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix bug in config files
</commit_message>
<xml_diff>
--- a/conf/excel/C_BackPolygon.xlsx
+++ b/conf/excel/C_BackPolygon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\File\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6B301D-F675-4EC9-92A2-45F43F1E5A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F788B-2BDF-4797-B9D1-6925687900E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1125" windowWidth="23580" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="3585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_BackPolygon.conf" sheetId="1" r:id="rId1"/>
@@ -630,10 +630,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>C_BackPolygon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>catalog=09020A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -658,187 +654,191 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>kind%=0136</t>
-  </si>
-  <si>
-    <t>kind%=0137</t>
-  </si>
-  <si>
-    <t>kind%=0133</t>
-  </si>
-  <si>
-    <t>kind%=0134</t>
-  </si>
-  <si>
-    <t>kind%=0121</t>
-  </si>
-  <si>
-    <t>kind%=0123;name=筒子河</t>
-  </si>
-  <si>
-    <t>#kind%=0123;dispclass=8</t>
-  </si>
-  <si>
-    <t>#kind%=0123;dispclass=7</t>
-  </si>
-  <si>
-    <t>kind%=0123;dispclass=5</t>
-  </si>
-  <si>
-    <t>kind%=0123;dispclass=4</t>
-  </si>
-  <si>
-    <t>kind%=0123;dispclass=3</t>
-  </si>
-  <si>
-    <t>kind%=0123;dispclass=2</t>
-  </si>
-  <si>
-    <t>kind%=0123;dispclass=1</t>
-  </si>
-  <si>
-    <t>kind%=0123</t>
-  </si>
-  <si>
-    <t>kind%=0122</t>
-  </si>
-  <si>
-    <t>kind%=0125</t>
-  </si>
-  <si>
-    <t>kind%=0143</t>
-  </si>
-  <si>
-    <t>kind%=0145</t>
-  </si>
-  <si>
-    <t>kind%=0146</t>
-  </si>
-  <si>
-    <t>kind%=0147</t>
-  </si>
-  <si>
-    <t>kind%=0148</t>
-  </si>
-  <si>
-    <t>scene_id&lt;InRange&gt;0001-0002;(kind%=0141 || kind%=014b || kind%=tx0160)</t>
-  </si>
-  <si>
-    <t>kind%=0141</t>
-  </si>
-  <si>
-    <t>kind%=0142</t>
-  </si>
-  <si>
-    <t>kind%=0144</t>
-  </si>
-  <si>
-    <t>kind%=0149</t>
-  </si>
-  <si>
-    <t>kind%=014a</t>
-  </si>
-  <si>
-    <t>kind%=014b</t>
-  </si>
-  <si>
-    <t>kind%=0161</t>
-  </si>
-  <si>
-    <t>kind%=0162</t>
-  </si>
-  <si>
-    <t>kind%=0163</t>
-  </si>
-  <si>
-    <t>kind%=0164</t>
-  </si>
-  <si>
-    <t>kind%=0165</t>
-  </si>
-  <si>
-    <t>kind%=0166</t>
-  </si>
-  <si>
-    <t>kind%=0167</t>
-  </si>
-  <si>
-    <t>kind%=0171</t>
-  </si>
-  <si>
-    <t>kind%=0172</t>
-  </si>
-  <si>
-    <t>kind%=0173</t>
-  </si>
-  <si>
-    <t>kind%=0174</t>
-  </si>
-  <si>
-    <t>kind%=0175</t>
-  </si>
-  <si>
-    <t>kind%=0176</t>
-  </si>
-  <si>
-    <t>kind%=0177</t>
-  </si>
-  <si>
-    <t>kind%=0178</t>
-  </si>
-  <si>
-    <t>kind%=0179</t>
-  </si>
-  <si>
-    <t>kind%=017a</t>
-  </si>
-  <si>
-    <t>kind%=84FF || kind%=84ff</t>
-  </si>
-  <si>
-    <t>kind%=07FF || kind%=07ff</t>
-  </si>
-  <si>
-    <t>kind%=010bj0101</t>
-  </si>
-  <si>
-    <t>kind%=010bj0102</t>
-  </si>
-  <si>
-    <t>kind%=0141 || kind%=014b || kind%=tx0160</t>
-  </si>
-  <si>
-    <t>kind%=tx1000</t>
-  </si>
-  <si>
-    <t>kind%=tx2010</t>
-  </si>
-  <si>
-    <t>kind%=tx2000</t>
-  </si>
-  <si>
-    <t>kind%=tx1020</t>
-  </si>
-  <si>
-    <t>kind%=tx1030</t>
-  </si>
-  <si>
-    <t>kind%=tx1040</t>
-  </si>
-  <si>
-    <t>kind%=tx1050</t>
-  </si>
-  <si>
-    <t>kind%=tx1031</t>
-  </si>
-  <si>
-    <t>kind%=tx1051</t>
-  </si>
-  <si>
-    <t>kind%=tx1070</t>
-  </si>
-  <si>
-    <t>kind%=tx1060</t>
+    <t>kind=0136</t>
+  </si>
+  <si>
+    <t>kind=0137</t>
+  </si>
+  <si>
+    <t>kind=0133</t>
+  </si>
+  <si>
+    <t>kind=0134</t>
+  </si>
+  <si>
+    <t>kind=0121</t>
+  </si>
+  <si>
+    <t>kind=0123;name=筒子河</t>
+  </si>
+  <si>
+    <t>#kind=0123;dispclass=8</t>
+  </si>
+  <si>
+    <t>#kind=0123;dispclass=7</t>
+  </si>
+  <si>
+    <t>kind=0123;dispclass=5</t>
+  </si>
+  <si>
+    <t>kind=0123;dispclass=4</t>
+  </si>
+  <si>
+    <t>kind=0123;dispclass=3</t>
+  </si>
+  <si>
+    <t>kind=0123;dispclass=2</t>
+  </si>
+  <si>
+    <t>kind=0123;dispclass=1</t>
+  </si>
+  <si>
+    <t>kind=0123</t>
+  </si>
+  <si>
+    <t>kind=0122</t>
+  </si>
+  <si>
+    <t>kind=0125</t>
+  </si>
+  <si>
+    <t>kind=0143</t>
+  </si>
+  <si>
+    <t>kind=0145</t>
+  </si>
+  <si>
+    <t>kind=0146</t>
+  </si>
+  <si>
+    <t>kind=0147</t>
+  </si>
+  <si>
+    <t>kind=0148</t>
+  </si>
+  <si>
+    <t>scene_id&lt;InRange&gt;0001-0002;(kind=0141 || kind=014b || kind=tx0160)</t>
+  </si>
+  <si>
+    <t>kind=0141</t>
+  </si>
+  <si>
+    <t>kind=0142</t>
+  </si>
+  <si>
+    <t>kind=0144</t>
+  </si>
+  <si>
+    <t>kind=0149</t>
+  </si>
+  <si>
+    <t>kind=014a</t>
+  </si>
+  <si>
+    <t>kind=014b</t>
+  </si>
+  <si>
+    <t>kind=0161</t>
+  </si>
+  <si>
+    <t>kind=0162</t>
+  </si>
+  <si>
+    <t>kind=0163</t>
+  </si>
+  <si>
+    <t>kind=0164</t>
+  </si>
+  <si>
+    <t>kind=0165</t>
+  </si>
+  <si>
+    <t>kind=0166</t>
+  </si>
+  <si>
+    <t>kind=0167</t>
+  </si>
+  <si>
+    <t>kind=0171</t>
+  </si>
+  <si>
+    <t>kind=0172</t>
+  </si>
+  <si>
+    <t>kind=0173</t>
+  </si>
+  <si>
+    <t>kind=0174</t>
+  </si>
+  <si>
+    <t>kind=0175</t>
+  </si>
+  <si>
+    <t>kind=0176</t>
+  </si>
+  <si>
+    <t>kind=0177</t>
+  </si>
+  <si>
+    <t>kind=0178</t>
+  </si>
+  <si>
+    <t>kind=0179</t>
+  </si>
+  <si>
+    <t>kind=017a</t>
+  </si>
+  <si>
+    <t>kind=84FF || kind=84ff</t>
+  </si>
+  <si>
+    <t>kind=07FF || kind=07ff</t>
+  </si>
+  <si>
+    <t>kind=010bj0101</t>
+  </si>
+  <si>
+    <t>kind=010bj0102</t>
+  </si>
+  <si>
+    <t>kind=0141 || kind=014b || kind=tx0160</t>
+  </si>
+  <si>
+    <t>kind=tx1000</t>
+  </si>
+  <si>
+    <t>kind=tx2010</t>
+  </si>
+  <si>
+    <t>kind=tx2000</t>
+  </si>
+  <si>
+    <t>kind=tx1020</t>
+  </si>
+  <si>
+    <t>kind=tx1030</t>
+  </si>
+  <si>
+    <t>kind=tx1040</t>
+  </si>
+  <si>
+    <t>kind=tx1050</t>
+  </si>
+  <si>
+    <t>kind=tx1031</t>
+  </si>
+  <si>
+    <t>kind=tx1051</t>
+  </si>
+  <si>
+    <t>kind=tx1070</t>
+  </si>
+  <si>
+    <t>kind=tx1060</t>
+  </si>
+  <si>
+    <t># C_BackPolygon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1270,7 +1270,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>159</v>
+        <v>226</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>21</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>23</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>152</v>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>153</v>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>15</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>19</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>25</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>8</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>29</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>31</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>33</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>37</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>39</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>40</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>42</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>44</v>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>46</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>48</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>48</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>52</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>54</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>56</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>58</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>60</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>60</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>63</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>65</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>67</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>69</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>70</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>72</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>74</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>74</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>77</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>79</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>70</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>82</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>84</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>128</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>129</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>25</v>
@@ -1999,10 +1999,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>139</v>
@@ -2010,10 +2010,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>140</v>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>141</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>142</v>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>143</v>
@@ -2054,10 +2054,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>144</v>
@@ -2065,7 +2065,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>131</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>132</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>133</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>134</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>135</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Fix bug in back polygon config file
</commit_message>
<xml_diff>
--- a/conf/excel/C_BackPolygon.xlsx
+++ b/conf/excel/C_BackPolygon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\File\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F788B-2BDF-4797-B9D1-6925687900E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FF2638-CF3C-4C21-823C-33BC7BF1980C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="3585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10725" yWindow="2040" windowWidth="23580" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_BackPolygon.conf" sheetId="1" r:id="rId1"/>
@@ -376,9 +376,6 @@
     <t>假想线</t>
   </si>
   <si>
-    <t>id=SHDSN0001</t>
-  </si>
-  <si>
     <t>catalog=09110101</t>
   </si>
   <si>
@@ -654,190 +651,255 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>kind=0136</t>
-  </si>
-  <si>
-    <t>kind=0137</t>
-  </si>
-  <si>
-    <t>kind=0133</t>
-  </si>
-  <si>
-    <t>kind=0134</t>
-  </si>
-  <si>
-    <t>kind=0121</t>
-  </si>
-  <si>
-    <t>kind=0123;name=筒子河</t>
-  </si>
-  <si>
-    <t>#kind=0123;dispclass=8</t>
-  </si>
-  <si>
-    <t>#kind=0123;dispclass=7</t>
-  </si>
-  <si>
-    <t>kind=0123;dispclass=5</t>
-  </si>
-  <si>
-    <t>kind=0123;dispclass=4</t>
-  </si>
-  <si>
-    <t>kind=0123;dispclass=3</t>
-  </si>
-  <si>
-    <t>kind=0123;dispclass=2</t>
-  </si>
-  <si>
-    <t>kind=0123;dispclass=1</t>
-  </si>
-  <si>
-    <t>kind=0123</t>
-  </si>
-  <si>
-    <t>kind=0122</t>
-  </si>
-  <si>
-    <t>kind=0125</t>
-  </si>
-  <si>
-    <t>kind=0143</t>
-  </si>
-  <si>
-    <t>kind=0145</t>
-  </si>
-  <si>
-    <t>kind=0146</t>
-  </si>
-  <si>
-    <t>kind=0147</t>
-  </si>
-  <si>
-    <t>kind=0148</t>
-  </si>
-  <si>
-    <t>scene_id&lt;InRange&gt;0001-0002;(kind=0141 || kind=014b || kind=tx0160)</t>
-  </si>
-  <si>
-    <t>kind=0141</t>
-  </si>
-  <si>
-    <t>kind=0142</t>
-  </si>
-  <si>
-    <t>kind=0144</t>
-  </si>
-  <si>
-    <t>kind=0149</t>
-  </si>
-  <si>
-    <t>kind=014a</t>
-  </si>
-  <si>
-    <t>kind=014b</t>
-  </si>
-  <si>
-    <t>kind=0161</t>
-  </si>
-  <si>
-    <t>kind=0162</t>
-  </si>
-  <si>
-    <t>kind=0163</t>
-  </si>
-  <si>
-    <t>kind=0164</t>
-  </si>
-  <si>
-    <t>kind=0165</t>
-  </si>
-  <si>
-    <t>kind=0166</t>
-  </si>
-  <si>
-    <t>kind=0167</t>
-  </si>
-  <si>
-    <t>kind=0171</t>
-  </si>
-  <si>
-    <t>kind=0172</t>
-  </si>
-  <si>
-    <t>kind=0173</t>
-  </si>
-  <si>
-    <t>kind=0174</t>
-  </si>
-  <si>
-    <t>kind=0175</t>
-  </si>
-  <si>
-    <t>kind=0176</t>
-  </si>
-  <si>
-    <t>kind=0177</t>
-  </si>
-  <si>
-    <t>kind=0178</t>
-  </si>
-  <si>
-    <t>kind=0179</t>
-  </si>
-  <si>
-    <t>kind=017a</t>
-  </si>
-  <si>
-    <t>kind=84FF || kind=84ff</t>
-  </si>
-  <si>
-    <t>kind=07FF || kind=07ff</t>
-  </si>
-  <si>
-    <t>kind=010bj0101</t>
-  </si>
-  <si>
-    <t>kind=010bj0102</t>
-  </si>
-  <si>
-    <t>kind=0141 || kind=014b || kind=tx0160</t>
-  </si>
-  <si>
-    <t>kind=tx1000</t>
-  </si>
-  <si>
-    <t>kind=tx2010</t>
-  </si>
-  <si>
-    <t>kind=tx2000</t>
-  </si>
-  <si>
-    <t>kind=tx1020</t>
-  </si>
-  <si>
-    <t>kind=tx1030</t>
-  </si>
-  <si>
-    <t>kind=tx1040</t>
-  </si>
-  <si>
-    <t>kind=tx1050</t>
-  </si>
-  <si>
-    <t>kind=tx1031</t>
-  </si>
-  <si>
-    <t>kind=tx1051</t>
-  </si>
-  <si>
-    <t>kind=tx1070</t>
-  </si>
-  <si>
-    <t>kind=tx1060</t>
-  </si>
-  <si>
     <t># C_BackPolygon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0136"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0137"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0133"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0134"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0121"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0123";name=筒子河</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#kind="0123";dispclass=8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#kind="0123";dispclass=7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0123";dispclass=5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0123";dispclass=4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0123";dispclass=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0123";dispclass=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0123";dispclass=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0123"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0122"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0125"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0143"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0145"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0146"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0147"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0148"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scene_id&lt;InRange&gt;0001-0002;(kind="0141" || kind="014b" || kind="tx0160")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0141"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0142"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0144"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0149"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="014a"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="014b"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0161"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0162"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0163"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0164"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0165"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0166"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0167"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0171"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0172"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0173"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0174"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0175"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0176"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0177"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0178"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0179"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="017a"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="84FF" || kind="84ff"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="07FF" || kind="07ff"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id=SHDSN0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="010bj0101"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="010bj0102"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="0141" || kind="014b" || kind="tx0160"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1000"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx2010"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx2000"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1020"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1030"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1040"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1050"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1031"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1051"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1070"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind="tx1060"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1257,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1270,7 +1332,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>226</v>
+        <v>164</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1345,7 +1407,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1364,7 +1426,7 @@
         <v>171</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>26</v>
@@ -1375,7 +1437,7 @@
         <v>172</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>26</v>
@@ -1529,7 +1591,7 @@
         <v>186</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>39</v>
@@ -1812,178 +1874,178 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1994,139 +2056,139 @@
         <v>25</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2161,7 +2223,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2186,24 +2248,24 @@
     </row>
     <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>